<commit_message>
fixes to runequest product types
</commit_message>
<xml_diff>
--- a/runequest/checklist.xlsx
+++ b/runequest/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/runequest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146FF0F2-F285-D443-9026-F6A13C26DDAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B273AFFE-657A-B147-B0A8-B661D46D18E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{36150B7F-B3AE-6D44-8C5E-EA8FC990432E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{36150B7F-B3AE-6D44-8C5E-EA8FC990432E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,7 +742,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -904,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -975,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>